<commit_message>
added validation set method for lda / qda
</commit_message>
<xml_diff>
--- a/csv/ldaqda/ldaqda_pc15_perfs.xlsx
+++ b/csv/ldaqda/ldaqda_pc15_perfs.xlsx
@@ -114,16 +114,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>0.16203703703703703</v>
+        <v>0.17592592592592593</v>
       </c>
       <c r="C2" t="n">
-        <v>0.040887781788554844</v>
+        <v>0.07790994062208381</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3472222222222222</v>
+        <v>0.33796296296296297</v>
       </c>
       <c r="E2" t="n">
-        <v>0.09582326839255743</v>
+        <v>0.05670115145331431</v>
       </c>
     </row>
   </sheetData>
@@ -191,7 +191,7 @@
         <v>0.0</v>
       </c>
       <c r="C3" t="n">
-        <v>35.0</v>
+        <v>34.0</v>
       </c>
       <c r="D3" t="n">
         <v>0.0</v>
@@ -200,10 +200,10 @@
         <v>0.0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="G3" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -220,10 +220,10 @@
         <v>30.0</v>
       </c>
       <c r="E4" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F4" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="G4" t="n">
         <v>1.0</v>
@@ -240,13 +240,13 @@
         <v>0.0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E5" t="n">
-        <v>31.0</v>
+        <v>29.0</v>
       </c>
       <c r="F5" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="G5" t="n">
         <v>1.0</v>
@@ -263,10 +263,10 @@
         <v>0.0</v>
       </c>
       <c r="D6" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="E6" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="F6" t="n">
         <v>28.0</v>
@@ -337,7 +337,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>24.0</v>
+        <v>19.0</v>
       </c>
       <c r="C2" t="n">
         <v>0.0</v>
@@ -352,7 +352,7 @@
         <v>0.0</v>
       </c>
       <c r="G2" t="n">
-        <v>11.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="3">
@@ -363,10 +363,10 @@
         <v>0.0</v>
       </c>
       <c r="C3" t="n">
-        <v>31.0</v>
+        <v>30.0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E3" t="n">
         <v>1.0</v>
@@ -383,22 +383,22 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C4" t="n">
         <v>0.0</v>
       </c>
       <c r="D4" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
       <c r="E4" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="F4" t="n">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
       <c r="G4" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="5">
@@ -406,7 +406,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="C5" t="n">
         <v>0.0</v>
@@ -415,13 +415,13 @@
         <v>1.0</v>
       </c>
       <c r="E5" t="n">
-        <v>25.0</v>
+        <v>21.0</v>
       </c>
       <c r="F5" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="G5" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="6">
@@ -435,16 +435,16 @@
         <v>0.0</v>
       </c>
       <c r="D6" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="E6" t="n">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
       <c r="F6" t="n">
-        <v>17.0</v>
+        <v>24.0</v>
       </c>
       <c r="G6" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
@@ -452,22 +452,22 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="D7" t="n">
         <v>1.0</v>
       </c>
       <c r="E7" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="F7" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G7" t="n">
-        <v>22.0</v>
+        <v>26.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>